<commit_message>
singleton and single entity number functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/SudokuBoard.xlsx
+++ b/src/main/resources/SudokuBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AShubtsik\IdeaProjects\SudokuSolver\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45CB3864-CAB2-4129-873E-42D16235C5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217A19CE-2402-4905-AA66-ACE4D05366D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5EFDB615-B115-4D3F-B6F3-9D02DA039988}"/>
+    <workbookView xWindow="9984" yWindow="2676" windowWidth="17280" windowHeight="8916" xr2:uid="{5EFDB615-B115-4D3F-B6F3-9D02DA039988}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,17 +405,17 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="9" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -424,152 +424,152 @@
         <v>0</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G1">
         <v>0</v>
       </c>
       <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -587,18 +587,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -607,71 +607,71 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
         <v>7</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9">
+      <c r="C9">
         <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I9">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>